<commit_message>
Added new table defining PersonID - Name
</commit_message>
<xml_diff>
--- a/Documentation/Rotations.xlsx
+++ b/Documentation/Rotations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicky\Documents\Advanced Software Engineering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicky\Documents\Advanced Software Engineering\TrinityWayFinders\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628981C0-665A-4C9E-B3CF-C5FE3143AFDB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B868AC3-8C8F-47D1-B460-2C0212ED5824}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{7BBFCC14-53F5-471E-9FD5-393828BAA0D3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="53">
   <si>
     <t>1,2</t>
   </si>
@@ -166,6 +166,30 @@
   </si>
   <si>
     <t>ScrumMaster Rotations</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Zihan</t>
+  </si>
+  <si>
+    <t>Yifan</t>
+  </si>
+  <si>
+    <t>Saad</t>
+  </si>
+  <si>
+    <t>Nicky</t>
+  </si>
+  <si>
+    <t>Arun</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>Person</t>
   </si>
 </sst>
 </file>
@@ -302,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -328,6 +352,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -646,7 +674,7 @@
   <dimension ref="A4:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -684,8 +712,12 @@
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="10"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="10"/>
+      <c r="F5" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>52</v>
+      </c>
       <c r="I5" s="9"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -1070,7 +1102,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="8:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F17" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="H17" s="2"/>
       <c r="I17" s="12" t="s">
         <v>35</v>
@@ -1095,7 +1133,13 @@
       </c>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="8:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F18" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="H18" s="2"/>
       <c r="I18" s="12" t="s">
         <v>36</v>
@@ -1119,7 +1163,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="8:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F19" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="H19" s="2"/>
       <c r="I19" s="12" t="s">
         <v>37</v>
@@ -1143,7 +1193,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="8:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F20" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>47</v>
+      </c>
       <c r="H20" s="2"/>
       <c r="I20" s="12" t="s">
         <v>38</v>
@@ -1167,7 +1223,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="8:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F21" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>48</v>
+      </c>
       <c r="H21" s="2"/>
       <c r="I21" s="12" t="s">
         <v>39</v>
@@ -1191,7 +1253,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="8:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F22" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>49</v>
+      </c>
       <c r="H22" s="2"/>
       <c r="I22" s="12" t="s">
         <v>40</v>
@@ -1215,7 +1283,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="8:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="6:16" x14ac:dyDescent="0.3">
       <c r="H23" s="2"/>
       <c r="I23" s="12" t="s">
         <v>41</v>
@@ -1239,7 +1307,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="8:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="6:16" x14ac:dyDescent="0.3">
       <c r="I24" s="13" t="s">
         <v>42</v>
       </c>

</xml_diff>